<commit_message>
a* 및 lua_tinker 추가
</commit_message>
<xml_diff>
--- a/Document/Char_Info.xlsx
+++ b/Document/Char_Info.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lincoln\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lincoln\Desktop\GSP_TermProject\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -502,7 +502,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -541,7 +541,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="C2">
         <v>100</v>
@@ -570,7 +570,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="C3">
         <v>200</v>
@@ -599,7 +599,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>170</v>
+        <v>300</v>
       </c>
       <c r="C4">
         <v>400</v>
@@ -628,7 +628,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>260</v>
+        <v>400</v>
       </c>
       <c r="C5">
         <v>800</v>
@@ -648,7 +648,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>370</v>
+        <v>500</v>
       </c>
       <c r="C6">
         <v>1600</v>
@@ -665,7 +665,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="C7">
         <v>3200</v>
@@ -682,7 +682,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>640</v>
+        <v>700</v>
       </c>
       <c r="C8">
         <v>6400</v>
@@ -696,7 +696,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>790</v>
+        <v>800</v>
       </c>
       <c r="C9">
         <v>12800</v>
@@ -710,7 +710,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>950</v>
+        <v>900</v>
       </c>
       <c r="C10">
         <v>25600</v>
@@ -724,7 +724,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>1020</v>
+        <v>1000</v>
       </c>
       <c r="C11">
         <v>51200</v>

</xml_diff>